<commit_message>
Up WDRV 192 kHz
</commit_message>
<xml_diff>
--- a/WebVars.xlsx
+++ b/WebVars.xlsx
@@ -2503,9 +2503,6 @@
     </r>
   </si>
   <si>
-    <t>Sample Rate, 1…20000 Гц,  вывод в dec формате.</t>
-  </si>
-  <si>
     <t>wdrv_port</t>
   </si>
   <si>
@@ -2589,9 +2586,6 @@
     </r>
   </si>
   <si>
-    <t>Старт вывода, Sample Rate, 1…20000 Гц</t>
-  </si>
-  <si>
     <r>
       <t>Wdrv_stop=</t>
     </r>
@@ -6359,6 +6353,12 @@
       </rPr>
       <t xml:space="preserve"> применяется маска установки всех параметров, кроме записи во flash и перезагрузки.</t>
     </r>
+  </si>
+  <si>
+    <t>Старт вывода, Sample Rate, 1…192000 Гц</t>
+  </si>
+  <si>
+    <t>Sample Rate, 1…192000 Гц,  вывод в dec формате.</t>
   </si>
 </sst>
 </file>
@@ -6652,6 +6652,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6661,16 +6667,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6682,7 +6679,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7011,34 +7011,34 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
@@ -7063,11 +7063,11 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
@@ -7097,33 +7097,33 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="5" t="s">
         <v>22</v>
       </c>
@@ -7183,11 +7183,11 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
@@ -7307,17 +7307,17 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="19"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="18"/>
-      <c r="C38" s="20"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="5" t="s">
         <v>64</v>
       </c>
@@ -7343,8 +7343,8 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="17"/>
-      <c r="C41" s="17" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14" t="s">
         <v>70</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -7352,8 +7352,8 @@
       </c>
     </row>
     <row r="42" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
       <c r="D42" s="5" t="s">
         <v>72</v>
       </c>
@@ -7368,17 +7368,17 @@
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="19"/>
+      <c r="C44" s="23"/>
       <c r="D44" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="18"/>
-      <c r="C45" s="20"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="24"/>
       <c r="D45" s="5" t="s">
         <v>77</v>
       </c>
@@ -7406,10 +7406,10 @@
       </c>
     </row>
     <row r="48" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="14" t="s">
         <v>85</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -7417,8 +7417,8 @@
       </c>
     </row>
     <row r="49" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
       <c r="D49" s="7" t="s">
         <v>87</v>
       </c>
@@ -7451,10 +7451,10 @@
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -7462,8 +7462,8 @@
       </c>
     </row>
     <row r="54" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
       <c r="D54" s="7" t="s">
         <v>97</v>
       </c>
@@ -7487,10 +7487,10 @@
       </c>
     </row>
     <row r="57" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C57" s="14" t="s">
         <v>103</v>
       </c>
       <c r="D57" s="1" t="s">
@@ -7498,8 +7498,8 @@
       </c>
     </row>
     <row r="58" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
       <c r="D58" s="7" t="s">
         <v>105</v>
       </c>
@@ -7514,10 +7514,10 @@
       </c>
     </row>
     <row r="60" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="14" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -7525,18 +7525,18 @@
       </c>
     </row>
     <row r="61" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
       <c r="D61" s="7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="16"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="18"/>
     </row>
     <row r="63" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="s">
@@ -7548,11 +7548,11 @@
       </c>
     </row>
     <row r="64" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="16"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="18"/>
     </row>
     <row r="65" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
@@ -7668,10 +7668,10 @@
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="14" t="s">
         <v>146</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -7679,17 +7679,17 @@
       </c>
     </row>
     <row r="77" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
       <c r="D77" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="78" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C78" s="14" t="s">
         <v>149</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -7697,10 +7697,10 @@
       </c>
     </row>
     <row r="79" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
       <c r="D79" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="80" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7722,11 +7722,11 @@
       </c>
     </row>
     <row r="82" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="C82" s="15"/>
-      <c r="D82" s="16"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="18"/>
     </row>
     <row r="83" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
@@ -7879,11 +7879,11 @@
       </c>
     </row>
     <row r="97" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="16"/>
+      <c r="C97" s="17"/>
+      <c r="D97" s="18"/>
     </row>
     <row r="98" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="3" t="s">
@@ -8029,11 +8029,11 @@
       </c>
     </row>
     <row r="111" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="14" t="s">
+      <c r="B111" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="C111" s="15"/>
-      <c r="D111" s="16"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="18"/>
     </row>
     <row r="112" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="3" t="s">
@@ -8054,11 +8054,11 @@
       </c>
     </row>
     <row r="114" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="14" t="s">
+      <c r="B114" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C114" s="15"/>
-      <c r="D114" s="16"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="18"/>
     </row>
     <row r="115" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
@@ -8079,11 +8079,11 @@
       </c>
     </row>
     <row r="117" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="14" t="s">
+      <c r="B117" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="C117" s="15"/>
-      <c r="D117" s="16"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="18"/>
     </row>
     <row r="118" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
@@ -8104,65 +8104,65 @@
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="17" t="s">
+      <c r="B120" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="C120" s="17"/>
+      <c r="C120" s="14"/>
       <c r="D120" s="1" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="121" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="18"/>
-      <c r="C121" s="18"/>
+      <c r="B121" s="15"/>
+      <c r="C121" s="15"/>
       <c r="D121" s="9" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="17" t="s">
+      <c r="B122" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="C122" s="17"/>
+      <c r="C122" s="14"/>
       <c r="D122" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="123" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="18"/>
-      <c r="C123" s="18"/>
+      <c r="B123" s="15"/>
+      <c r="C123" s="15"/>
       <c r="D123" s="9" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="17" t="s">
+      <c r="B124" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="C124" s="17"/>
+      <c r="C124" s="14"/>
       <c r="D124" s="1" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="125" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="18"/>
-      <c r="C125" s="18"/>
+      <c r="B125" s="15"/>
+      <c r="C125" s="15"/>
       <c r="D125" s="9" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="17" t="s">
+      <c r="B126" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="C126" s="17"/>
+      <c r="C126" s="14"/>
       <c r="D126" s="1" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="127" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="18"/>
-      <c r="C127" s="18"/>
+      <c r="B127" s="15"/>
+      <c r="C127" s="15"/>
       <c r="D127" s="9" t="s">
         <v>241</v>
       </c>
@@ -8186,11 +8186,11 @@
       </c>
     </row>
     <row r="130" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="14" t="s">
+      <c r="B130" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="C130" s="15"/>
-      <c r="D130" s="16"/>
+      <c r="C130" s="17"/>
+      <c r="D130" s="18"/>
     </row>
     <row r="131" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
@@ -8229,11 +8229,11 @@
       </c>
     </row>
     <row r="135" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="21" t="s">
+      <c r="B135" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="C135" s="22"/>
-      <c r="D135" s="23"/>
+      <c r="C135" s="21"/>
+      <c r="D135" s="22"/>
     </row>
     <row r="136" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
@@ -8243,1138 +8243,1138 @@
         <v>263</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>264</v>
+        <v>473</v>
       </c>
     </row>
     <row r="137" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C137" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="C137" s="4" t="s">
+      <c r="D137" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="D137" s="5" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="138" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C138" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="D138" s="5" t="s">
         <v>269</v>
-      </c>
-      <c r="D138" s="5" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="139" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B139" s="3"/>
       <c r="C139" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D139" s="5" t="s">
         <v>271</v>
-      </c>
-      <c r="D139" s="5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="140" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B140" s="3"/>
       <c r="C140" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>274</v>
+        <v>472</v>
       </c>
     </row>
     <row r="141" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B141" s="3"/>
       <c r="C141" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="D141" s="5" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="142" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="C142" s="15"/>
-      <c r="D142" s="16"/>
+      <c r="C142" s="17"/>
+      <c r="D142" s="18"/>
     </row>
     <row r="143" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C143" s="4"/>
       <c r="D143" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="C144" s="17"/>
+      <c r="D144" s="18"/>
+    </row>
+    <row r="145" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B145" s="14" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="144" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="14" t="s">
+      <c r="C145" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="C144" s="15"/>
-      <c r="D144" s="16"/>
-    </row>
-    <row r="145" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B145" s="17" t="s">
+      <c r="D145" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C145" s="17" t="s">
+    </row>
+    <row r="146" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B146" s="15"/>
+      <c r="C146" s="15"/>
+      <c r="D146" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="D145" s="1" t="s">
+    </row>
+    <row r="147" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B147" s="14" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="146" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="18"/>
-      <c r="C146" s="18"/>
-      <c r="D146" s="7" t="s">
+      <c r="C147" s="14" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="147" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B147" s="17" t="s">
+      <c r="D147" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C147" s="17" t="s">
+    </row>
+    <row r="148" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B148" s="15"/>
+      <c r="C148" s="15"/>
+      <c r="D148" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B149" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="C149" s="14" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="148" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="18"/>
-      <c r="C148" s="18"/>
-      <c r="D148" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="149" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B149" s="17" t="s">
+      <c r="D149" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C149" s="17" t="s">
+    </row>
+    <row r="150" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="15"/>
+      <c r="C150" s="15"/>
+      <c r="D150" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="14"/>
+      <c r="C151" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="D149" s="1" t="s">
+      <c r="D151" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="150" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="18"/>
-      <c r="C150" s="18"/>
-      <c r="D150" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="17"/>
-      <c r="C151" s="17" t="s">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="19"/>
+      <c r="C152" s="19"/>
+      <c r="D152" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="D151" s="1" t="s">
+    </row>
+    <row r="153" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="15"/>
+      <c r="C153" s="15"/>
+      <c r="D153" s="9" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="24"/>
-      <c r="C152" s="24"/>
-      <c r="D152" s="10" t="s">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="14"/>
+      <c r="C154" s="14" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="153" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="18"/>
-      <c r="C153" s="18"/>
-      <c r="D153" s="9" t="s">
+      <c r="D154" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="17"/>
-      <c r="C154" s="17" t="s">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="19"/>
+      <c r="C155" s="19"/>
+      <c r="D155" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="15"/>
+      <c r="C156" s="15"/>
+      <c r="D156" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="C157" s="14"/>
+      <c r="D157" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="D154" s="1" t="s">
+    </row>
+    <row r="158" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B158" s="15"/>
+      <c r="C158" s="15"/>
+      <c r="D158" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="C159" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="24"/>
-      <c r="C155" s="24"/>
-      <c r="D155" s="10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="156" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="18"/>
-      <c r="C156" s="18"/>
-      <c r="D156" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="17" t="s">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="19"/>
+      <c r="C160" s="19"/>
+      <c r="D160" s="10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B161" s="15"/>
+      <c r="C161" s="15"/>
+      <c r="D161" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="14"/>
+      <c r="C162" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="19"/>
+      <c r="C163" s="19"/>
+      <c r="D163" s="10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B164" s="15"/>
+      <c r="C164" s="15"/>
+      <c r="D164" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="14"/>
+      <c r="C165" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="19"/>
+      <c r="C166" s="19"/>
+      <c r="D166" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B167" s="15"/>
+      <c r="C167" s="15"/>
+      <c r="D167" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="14" t="s">
         <v>450</v>
       </c>
-      <c r="C157" s="17"/>
-      <c r="D157" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="158" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="18"/>
-      <c r="C158" s="18"/>
-      <c r="D158" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="17" t="s">
+      <c r="C168" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="19"/>
+      <c r="C169" s="19"/>
+      <c r="D169" s="10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="15"/>
+      <c r="C170" s="15"/>
+      <c r="D170" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="14"/>
+      <c r="C171" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="15"/>
+      <c r="C172" s="15"/>
+      <c r="D172" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="14"/>
+      <c r="C173" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="15"/>
+      <c r="C174" s="15"/>
+      <c r="D174" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="14" t="s">
         <v>451</v>
       </c>
-      <c r="C159" s="17" t="s">
-        <v>458</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="24"/>
-      <c r="C160" s="24"/>
-      <c r="D160" s="10" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="161" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="18"/>
-      <c r="C161" s="18"/>
-      <c r="D161" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="17"/>
-      <c r="C162" s="17" t="s">
-        <v>459</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="24"/>
-      <c r="C163" s="24"/>
-      <c r="D163" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="18"/>
-      <c r="C164" s="18"/>
-      <c r="D164" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="17"/>
-      <c r="C165" s="17" t="s">
-        <v>460</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="24"/>
-      <c r="C166" s="24"/>
-      <c r="D166" s="10" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="167" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="18"/>
-      <c r="C167" s="18"/>
-      <c r="D167" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="17" t="s">
+      <c r="C175" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="19"/>
+      <c r="C176" s="19"/>
+      <c r="D176" s="10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B177" s="15"/>
+      <c r="C177" s="15"/>
+      <c r="D177" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="C168" s="17" t="s">
-        <v>461</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="24"/>
-      <c r="C169" s="24"/>
-      <c r="D169" s="10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="18"/>
-      <c r="C170" s="18"/>
-      <c r="D170" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="17"/>
-      <c r="C171" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="18"/>
-      <c r="C172" s="18"/>
-      <c r="D172" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="17"/>
-      <c r="C173" s="17" t="s">
+      <c r="C178" s="14"/>
+      <c r="D178" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="19"/>
+      <c r="C179" s="19"/>
+      <c r="D179" s="10" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="15"/>
+      <c r="C180" s="15"/>
+      <c r="D180" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="C181" s="14" t="s">
         <v>463</v>
       </c>
-      <c r="D173" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="174" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="18"/>
-      <c r="C174" s="18"/>
-      <c r="D174" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="17" t="s">
-        <v>453</v>
-      </c>
-      <c r="C175" s="17" t="s">
+      <c r="D181" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="19"/>
+      <c r="C182" s="19"/>
+      <c r="D182" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="15"/>
+      <c r="C183" s="15"/>
+      <c r="D183" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B184" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="C184" s="14" t="s">
         <v>464</v>
       </c>
-      <c r="D175" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B176" s="24"/>
-      <c r="C176" s="24"/>
-      <c r="D176" s="10" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="177" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="18"/>
-      <c r="C177" s="18"/>
-      <c r="D177" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B178" s="17" t="s">
-        <v>454</v>
-      </c>
-      <c r="C178" s="17"/>
-      <c r="D178" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="24"/>
-      <c r="C179" s="24"/>
-      <c r="D179" s="10" t="s">
+      <c r="D184" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B185" s="19"/>
+      <c r="C185" s="19"/>
+      <c r="D185" s="10" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="180" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="18"/>
-      <c r="C180" s="18"/>
-      <c r="D180" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" s="17" t="s">
+    <row r="186" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B186" s="15"/>
+      <c r="C186" s="15"/>
+      <c r="D186" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B187" s="14" t="s">
         <v>455</v>
       </c>
-      <c r="C181" s="17" t="s">
+      <c r="C187" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="D181" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="24"/>
-      <c r="C182" s="24"/>
-      <c r="D182" s="10" t="s">
+      <c r="D187" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="183" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="18"/>
-      <c r="C183" s="18"/>
-      <c r="D183" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="17" t="s">
-        <v>456</v>
-      </c>
-      <c r="C184" s="17" t="s">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B188" s="19"/>
+      <c r="C188" s="19"/>
+      <c r="D188" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B189" s="15"/>
+      <c r="C189" s="15"/>
+      <c r="D189" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="14"/>
+      <c r="C190" s="14" t="s">
         <v>466</v>
       </c>
-      <c r="D184" s="1" t="s">
+      <c r="D190" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="24"/>
-      <c r="C185" s="24"/>
-      <c r="D185" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="186" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B186" s="18"/>
-      <c r="C186" s="18"/>
-      <c r="D186" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B187" s="17" t="s">
-        <v>457</v>
-      </c>
-      <c r="C187" s="17" t="s">
+    <row r="191" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B191" s="15"/>
+      <c r="C191" s="15"/>
+      <c r="D191" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B192" s="14"/>
+      <c r="C192" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="D187" s="1" t="s">
+      <c r="D192" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B188" s="24"/>
-      <c r="C188" s="24"/>
-      <c r="D188" s="10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="189" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B189" s="18"/>
-      <c r="C189" s="18"/>
-      <c r="D189" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B190" s="17"/>
-      <c r="C190" s="17" t="s">
+    <row r="193" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="15"/>
+      <c r="C193" s="15"/>
+      <c r="D193" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194" s="14"/>
+      <c r="C194" s="14" t="s">
         <v>468</v>
       </c>
-      <c r="D190" s="1" t="s">
+      <c r="D194" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="191" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="18"/>
-      <c r="C191" s="18"/>
-      <c r="D191" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B192" s="17"/>
-      <c r="C192" s="17" t="s">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" s="19"/>
+      <c r="C195" s="19"/>
+      <c r="D195" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="15"/>
+      <c r="C196" s="15"/>
+      <c r="D196" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="14"/>
+      <c r="C197" s="14" t="s">
         <v>469</v>
       </c>
-      <c r="D192" s="1" t="s">
+      <c r="D197" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B198" s="15"/>
+      <c r="C198" s="15"/>
+      <c r="D198" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B199" s="14"/>
+      <c r="C199" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="15"/>
+      <c r="C200" s="15"/>
+      <c r="D200" s="9" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="193" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B193" s="18"/>
-      <c r="C193" s="18"/>
-      <c r="D193" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B194" s="17"/>
-      <c r="C194" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="24"/>
-      <c r="C195" s="24"/>
-      <c r="D195" s="10" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="196" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="18"/>
-      <c r="C196" s="18"/>
-      <c r="D196" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B197" s="17"/>
-      <c r="C197" s="17" t="s">
-        <v>471</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="198" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B198" s="18"/>
-      <c r="C198" s="18"/>
-      <c r="D198" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B199" s="17"/>
-      <c r="C199" s="17" t="s">
+    <row r="201" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B201" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="D199" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="18"/>
-      <c r="C200" s="18"/>
-      <c r="D200" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="201" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="C201" s="15"/>
-      <c r="D201" s="16"/>
+      <c r="C201" s="17"/>
+      <c r="D201" s="18"/>
     </row>
     <row r="202" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B202" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D202" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="C202" s="4" t="s">
+    </row>
+    <row r="203" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B203" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="D202" s="5" t="s">
+      <c r="C203" s="14" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="203" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B203" s="17" t="s">
+      <c r="D203" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B204" s="15"/>
+      <c r="C204" s="15"/>
+      <c r="D204" s="9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B205" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="C203" s="17" t="s">
+      <c r="C205" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="D203" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="204" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="18"/>
-      <c r="C204" s="18"/>
-      <c r="D204" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="205" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B205" s="17" t="s">
+      <c r="D205" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C205" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>331</v>
-      </c>
     </row>
     <row r="206" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B206" s="18"/>
-      <c r="C206" s="18"/>
+      <c r="B206" s="15"/>
+      <c r="C206" s="15"/>
       <c r="D206" s="9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="207" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B207" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D207" s="5" t="s">
         <v>332</v>
-      </c>
-      <c r="C207" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="D207" s="5" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="208" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B208" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D208" s="5" t="s">
         <v>335</v>
-      </c>
-      <c r="C208" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="D208" s="5" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="209" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B209" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D209" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="C209" s="4" t="s">
+    </row>
+    <row r="210" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B210" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="D209" s="5" t="s">
+      <c r="C210" s="14" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="210" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B210" s="17" t="s">
+      <c r="D210" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B211" s="15"/>
+      <c r="C211" s="15"/>
+      <c r="D211" s="9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B212" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="C210" s="17" t="s">
+      <c r="C212" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="D210" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="211" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B211" s="18"/>
-      <c r="C211" s="18"/>
-      <c r="D211" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="212" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B212" s="17" t="s">
+      <c r="D212" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C212" s="17" t="s">
-        <v>344</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>345</v>
-      </c>
     </row>
     <row r="213" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B213" s="18"/>
-      <c r="C213" s="18"/>
+      <c r="B213" s="15"/>
+      <c r="C213" s="15"/>
       <c r="D213" s="9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="214" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B214" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="D214" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="C214" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D214" s="5" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="215" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B215" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D215" s="5" t="s">
         <v>349</v>
-      </c>
-      <c r="C215" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="D215" s="5" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="216" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B216" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D216" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="C216" s="4" t="s">
+    </row>
+    <row r="217" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B217" s="14" t="s">
         <v>353</v>
       </c>
-      <c r="D216" s="5" t="s">
+      <c r="C217" s="14" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="217" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B217" s="17" t="s">
+      <c r="D217" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="218" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B218" s="15"/>
+      <c r="C218" s="15"/>
+      <c r="D218" s="9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B219" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="C217" s="17" t="s">
+      <c r="C219" s="14" t="s">
         <v>356</v>
       </c>
-      <c r="D217" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="218" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B218" s="18"/>
-      <c r="C218" s="18"/>
-      <c r="D218" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="219" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B219" s="17" t="s">
+      <c r="D219" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C219" s="17" t="s">
-        <v>358</v>
-      </c>
-      <c r="D219" s="1" t="s">
-        <v>359</v>
-      </c>
     </row>
     <row r="220" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B220" s="18"/>
-      <c r="C220" s="18"/>
+      <c r="B220" s="15"/>
+      <c r="C220" s="15"/>
       <c r="D220" s="9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="221" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B221" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D221" s="5" t="s">
         <v>360</v>
-      </c>
-      <c r="C221" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="D221" s="5" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="222" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B222" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D222" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="C222" s="4" t="s">
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B223" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="D222" s="5" t="s">
+      <c r="C223" s="14" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B223" s="17" t="s">
+      <c r="D223" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C223" s="17" t="s">
+    </row>
+    <row r="224" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B224" s="15"/>
+      <c r="C224" s="15"/>
+      <c r="D224" s="5" t="s">
         <v>367</v>
-      </c>
-      <c r="D223" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="224" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B224" s="18"/>
-      <c r="C224" s="18"/>
-      <c r="D224" s="5" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="225" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B225" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="D225" s="5" t="s">
         <v>370</v>
-      </c>
-      <c r="C225" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="D225" s="5" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="226" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B226" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D226" s="5" t="s">
         <v>373</v>
-      </c>
-      <c r="C226" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="D226" s="5" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="227" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B227" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D227" s="5" t="s">
         <v>376</v>
-      </c>
-      <c r="C227" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="D227" s="5" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="228" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B228" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C228" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D228" s="5" t="s">
         <v>379</v>
-      </c>
-      <c r="C228" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="D228" s="5" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="229" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B229" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C229" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="D229" s="5" t="s">
         <v>382</v>
-      </c>
-      <c r="C229" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D229" s="5" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="230" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B230" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C230" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="D230" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="C230" s="4" t="s">
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B231" s="14"/>
+      <c r="C231" s="14" t="s">
         <v>386</v>
       </c>
-      <c r="D230" s="5" t="s">
+      <c r="D231" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B231" s="17"/>
-      <c r="C231" s="17" t="s">
+    <row r="232" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B232" s="15"/>
+      <c r="C232" s="15"/>
+      <c r="D232" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="D231" s="1" t="s">
+    </row>
+    <row r="233" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B233" s="16" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="232" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B232" s="18"/>
-      <c r="C232" s="18"/>
-      <c r="D232" s="5" t="s">
+      <c r="C233" s="17"/>
+      <c r="D233" s="18"/>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B234" s="14" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="233" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B233" s="14" t="s">
+      <c r="C234" s="14" t="s">
         <v>391</v>
       </c>
-      <c r="C233" s="15"/>
-      <c r="D233" s="16"/>
-    </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B234" s="17" t="s">
+      <c r="D234" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="C234" s="17" t="s">
+    </row>
+    <row r="235" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B235" s="15"/>
+      <c r="C235" s="15"/>
+      <c r="D235" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="D234" s="1" t="s">
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B236" s="14" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="235" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B235" s="18"/>
-      <c r="C235" s="18"/>
-      <c r="D235" s="9" t="s">
+      <c r="C236" s="14" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B236" s="17" t="s">
+      <c r="D236" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C236" s="17" t="s">
+    </row>
+    <row r="237" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B237" s="15"/>
+      <c r="C237" s="15"/>
+      <c r="D237" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="D236" s="1" t="s">
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B238" s="14" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="237" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B237" s="18"/>
-      <c r="C237" s="18"/>
-      <c r="D237" s="9" t="s">
+      <c r="C238" s="14" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B238" s="17" t="s">
+      <c r="D238" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="C238" s="17" t="s">
+    </row>
+    <row r="239" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B239" s="15"/>
+      <c r="C239" s="15"/>
+      <c r="D239" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="D238" s="1" t="s">
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B240" s="14" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="239" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B239" s="18"/>
-      <c r="C239" s="18"/>
-      <c r="D239" s="9" t="s">
+      <c r="C240" s="14" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B240" s="17" t="s">
+      <c r="D240" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="C240" s="17" t="s">
+    </row>
+    <row r="241" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B241" s="15"/>
+      <c r="C241" s="15"/>
+      <c r="D241" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="D240" s="1" t="s">
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B242" s="14" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="241" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B241" s="18"/>
-      <c r="C241" s="18"/>
-      <c r="D241" s="9" t="s">
+      <c r="C242" s="14" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B242" s="17" t="s">
+      <c r="D242" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="C242" s="17" t="s">
+    </row>
+    <row r="243" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B243" s="15"/>
+      <c r="C243" s="15"/>
+      <c r="D243" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="D242" s="1" t="s">
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B244" s="14" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="243" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B243" s="18"/>
-      <c r="C243" s="18"/>
-      <c r="D243" s="9" t="s">
+      <c r="C244" s="14" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B244" s="17" t="s">
+      <c r="D244" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="C244" s="17" t="s">
+    </row>
+    <row r="245" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B245" s="15"/>
+      <c r="C245" s="15"/>
+      <c r="D245" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B246" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="D244" s="1" t="s">
+      <c r="C246" s="14" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="245" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B245" s="18"/>
-      <c r="C245" s="18"/>
-      <c r="D245" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B246" s="17" t="s">
+      <c r="D246" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="C246" s="17" t="s">
+    </row>
+    <row r="247" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B247" s="15"/>
+      <c r="C247" s="15"/>
+      <c r="D247" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B248" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="D246" s="1" t="s">
+      <c r="C248" s="14" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="247" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B247" s="18"/>
-      <c r="C247" s="18"/>
-      <c r="D247" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B248" s="17" t="s">
+      <c r="D248" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C248" s="17" t="s">
+    </row>
+    <row r="249" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B249" s="15"/>
+      <c r="C249" s="15"/>
+      <c r="D249" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B250" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="D248" s="1" t="s">
+      <c r="C250" s="14" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="249" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B249" s="18"/>
-      <c r="C249" s="18"/>
-      <c r="D249" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B250" s="17" t="s">
+      <c r="D250" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="C250" s="17" t="s">
+    </row>
+    <row r="251" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B251" s="15"/>
+      <c r="C251" s="15"/>
+      <c r="D251" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B252" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="D250" s="1" t="s">
+      <c r="C252" s="14" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="251" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B251" s="18"/>
-      <c r="C251" s="18"/>
-      <c r="D251" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B252" s="17" t="s">
+      <c r="D252" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C252" s="17" t="s">
+    </row>
+    <row r="253" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B253" s="15"/>
+      <c r="C253" s="15"/>
+      <c r="D253" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B254" s="14" t="s">
         <v>425</v>
       </c>
-      <c r="D252" s="1" t="s">
+      <c r="C254" s="14" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="253" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B253" s="18"/>
-      <c r="C253" s="18"/>
-      <c r="D253" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B254" s="17" t="s">
+      <c r="D254" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="C254" s="17" t="s">
+    </row>
+    <row r="255" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B255" s="15"/>
+      <c r="C255" s="15"/>
+      <c r="D255" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B256" s="14" t="s">
         <v>428</v>
       </c>
-      <c r="D254" s="1" t="s">
+      <c r="C256" s="14" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="255" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B255" s="18"/>
-      <c r="C255" s="18"/>
-      <c r="D255" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B256" s="17" t="s">
+      <c r="D256" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C256" s="17" t="s">
+    </row>
+    <row r="257" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B257" s="15"/>
+      <c r="C257" s="15"/>
+      <c r="D257" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B258" s="14" t="s">
         <v>431</v>
       </c>
-      <c r="D256" s="1" t="s">
+      <c r="C258" s="14" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="257" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B257" s="18"/>
-      <c r="C257" s="18"/>
-      <c r="D257" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B258" s="17" t="s">
+      <c r="D258" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="C258" s="17" t="s">
+    </row>
+    <row r="259" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B259" s="15"/>
+      <c r="C259" s="15"/>
+      <c r="D259" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B260" s="14" t="s">
         <v>434</v>
       </c>
-      <c r="D258" s="1" t="s">
+      <c r="C260" s="14" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="259" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B259" s="18"/>
-      <c r="C259" s="18"/>
-      <c r="D259" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B260" s="17" t="s">
+      <c r="D260" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C260" s="17" t="s">
+    </row>
+    <row r="261" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B261" s="15"/>
+      <c r="C261" s="15"/>
+      <c r="D261" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B262" s="14"/>
+      <c r="C262" s="14" t="s">
         <v>437</v>
       </c>
-      <c r="D260" s="1" t="s">
+      <c r="D262" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="261" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B261" s="18"/>
-      <c r="C261" s="18"/>
-      <c r="D261" s="9" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B262" s="17"/>
-      <c r="C262" s="17" t="s">
+    <row r="263" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B263" s="15"/>
+      <c r="C263" s="15"/>
+      <c r="D263" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="D262" s="1" t="s">
+    </row>
+    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B264" s="14"/>
+      <c r="C264" s="14" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="263" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B263" s="18"/>
-      <c r="C263" s="18"/>
-      <c r="D263" s="5" t="s">
+      <c r="D264" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B264" s="17"/>
-      <c r="C264" s="17" t="s">
-        <v>442</v>
-      </c>
-      <c r="D264" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
     <row r="265" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B265" s="18"/>
-      <c r="C265" s="18"/>
+      <c r="B265" s="15"/>
+      <c r="C265" s="15"/>
       <c r="D265" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="266" spans="2:4" x14ac:dyDescent="0.25">
@@ -9382,28 +9382,112 @@
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="B262:B263"/>
-    <mergeCell ref="C262:C263"/>
-    <mergeCell ref="B264:B265"/>
-    <mergeCell ref="C264:C265"/>
-    <mergeCell ref="B256:B257"/>
-    <mergeCell ref="C256:C257"/>
-    <mergeCell ref="B258:B259"/>
-    <mergeCell ref="C258:C259"/>
-    <mergeCell ref="B260:B261"/>
-    <mergeCell ref="C260:C261"/>
-    <mergeCell ref="B250:B251"/>
-    <mergeCell ref="C250:C251"/>
-    <mergeCell ref="B252:B253"/>
-    <mergeCell ref="C252:C253"/>
-    <mergeCell ref="B254:B255"/>
-    <mergeCell ref="C254:C255"/>
-    <mergeCell ref="B244:B245"/>
-    <mergeCell ref="C244:C245"/>
-    <mergeCell ref="B246:B247"/>
-    <mergeCell ref="C246:C247"/>
-    <mergeCell ref="B248:B249"/>
-    <mergeCell ref="C248:C249"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="B135:D135"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="C151:C153"/>
+    <mergeCell ref="B154:B156"/>
+    <mergeCell ref="C154:C156"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="B144:D144"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="B165:B167"/>
+    <mergeCell ref="C165:C167"/>
+    <mergeCell ref="B168:B170"/>
+    <mergeCell ref="C168:C170"/>
+    <mergeCell ref="B171:B172"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="C157:C158"/>
+    <mergeCell ref="B159:B161"/>
+    <mergeCell ref="C159:C161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="C162:C164"/>
+    <mergeCell ref="B181:B183"/>
+    <mergeCell ref="C181:C183"/>
+    <mergeCell ref="B184:B186"/>
+    <mergeCell ref="C184:C186"/>
+    <mergeCell ref="B187:B189"/>
+    <mergeCell ref="C187:C189"/>
+    <mergeCell ref="B173:B174"/>
+    <mergeCell ref="C173:C174"/>
+    <mergeCell ref="B175:B177"/>
+    <mergeCell ref="C175:C177"/>
+    <mergeCell ref="B178:B180"/>
+    <mergeCell ref="C178:C180"/>
+    <mergeCell ref="B197:B198"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="B199:B200"/>
+    <mergeCell ref="C199:C200"/>
+    <mergeCell ref="B201:D201"/>
+    <mergeCell ref="B203:B204"/>
+    <mergeCell ref="C203:C204"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="C190:C191"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="B194:B196"/>
+    <mergeCell ref="C194:C196"/>
+    <mergeCell ref="B217:B218"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="B219:B220"/>
+    <mergeCell ref="C219:C220"/>
+    <mergeCell ref="B223:B224"/>
+    <mergeCell ref="C223:C224"/>
+    <mergeCell ref="B205:B206"/>
+    <mergeCell ref="C205:C206"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:C211"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:C213"/>
     <mergeCell ref="B238:B239"/>
     <mergeCell ref="C238:C239"/>
     <mergeCell ref="B240:B241"/>
@@ -9417,112 +9501,28 @@
     <mergeCell ref="C234:C235"/>
     <mergeCell ref="B236:B237"/>
     <mergeCell ref="C236:C237"/>
-    <mergeCell ref="B217:B218"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="B219:B220"/>
-    <mergeCell ref="C219:C220"/>
-    <mergeCell ref="B223:B224"/>
-    <mergeCell ref="C223:C224"/>
-    <mergeCell ref="B205:B206"/>
-    <mergeCell ref="C205:C206"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:C211"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:C213"/>
-    <mergeCell ref="B197:B198"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="B199:B200"/>
-    <mergeCell ref="C199:C200"/>
-    <mergeCell ref="B201:D201"/>
-    <mergeCell ref="B203:B204"/>
-    <mergeCell ref="C203:C204"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="C190:C191"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="B194:B196"/>
-    <mergeCell ref="C194:C196"/>
-    <mergeCell ref="B181:B183"/>
-    <mergeCell ref="C181:C183"/>
-    <mergeCell ref="B184:B186"/>
-    <mergeCell ref="C184:C186"/>
-    <mergeCell ref="B187:B189"/>
-    <mergeCell ref="C187:C189"/>
-    <mergeCell ref="B173:B174"/>
-    <mergeCell ref="C173:C174"/>
-    <mergeCell ref="B175:B177"/>
-    <mergeCell ref="C175:C177"/>
-    <mergeCell ref="B178:B180"/>
-    <mergeCell ref="C178:C180"/>
-    <mergeCell ref="B165:B167"/>
-    <mergeCell ref="C165:C167"/>
-    <mergeCell ref="B168:B170"/>
-    <mergeCell ref="C168:C170"/>
-    <mergeCell ref="B171:B172"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="B159:B161"/>
-    <mergeCell ref="C159:C161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="C162:C164"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="B151:B153"/>
-    <mergeCell ref="C151:C153"/>
-    <mergeCell ref="B154:B156"/>
-    <mergeCell ref="C154:C156"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="B144:D144"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="B135:D135"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B250:B251"/>
+    <mergeCell ref="C250:C251"/>
+    <mergeCell ref="B252:B253"/>
+    <mergeCell ref="C252:C253"/>
+    <mergeCell ref="B254:B255"/>
+    <mergeCell ref="C254:C255"/>
+    <mergeCell ref="B244:B245"/>
+    <mergeCell ref="C244:C245"/>
+    <mergeCell ref="B246:B247"/>
+    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="B248:B249"/>
+    <mergeCell ref="C248:C249"/>
+    <mergeCell ref="B262:B263"/>
+    <mergeCell ref="C262:C263"/>
+    <mergeCell ref="B264:B265"/>
+    <mergeCell ref="C264:C265"/>
+    <mergeCell ref="B256:B257"/>
+    <mergeCell ref="C256:C257"/>
+    <mergeCell ref="B258:B259"/>
+    <mergeCell ref="C258:C259"/>
+    <mergeCell ref="B260:B261"/>
+    <mergeCell ref="C260:C261"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>